<commit_message>
Fix EffortLog_W10 and ConceptofOperation
</commit_message>
<xml_diff>
--- a/8. EffortLog/8.5 Minh Doan/MinhDoan-EffortLog-W10.xlsx
+++ b/8. EffortLog/8.5 Minh Doan/MinhDoan-EffortLog-W10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>NO</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Concepts Of Operation</t>
+  </si>
+  <si>
+    <t>Meeting with customer</t>
+  </si>
+  <si>
+    <t>Usecase Description</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -578,17 +584,17 @@
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8">
+        <v>42533</v>
+      </c>
+      <c r="F5" s="7">
         <v>6</v>
       </c>
-      <c r="E5" s="6">
-        <v>42594</v>
-      </c>
-      <c r="F5" s="5">
-        <v>5</v>
-      </c>
-      <c r="G5" s="5">
-        <v>6</v>
+      <c r="G5" s="7">
+        <v>2</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -613,11 +619,21 @@
     <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6">
+        <v>42594</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>6</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -641,11 +657,21 @@
     <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6">
+        <v>42625</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -923,10 +949,6 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -951,10 +973,6 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>

</xml_diff>